<commit_message>
Update ClassDiagram, ERD, 테이블설계서
</commit_message>
<xml_diff>
--- a/02.설계/StudyStory 테이블설계서_v0404.xlsx
+++ b/02.설계/StudyStory 테이블설계서_v0404.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="22575" windowHeight="6210" tabRatio="862" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="22575" windowHeight="6210" tabRatio="862" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -1846,6 +1846,98 @@
         </r>
       </text>
     </comment>
+    <comment ref="G11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>답변</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>등록</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>시</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> SYSDATE</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">처리
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -3254,6 +3346,192 @@
         </r>
       </text>
     </comment>
+    <comment ref="G14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>delete:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>새</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>스터디에</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>취소되면</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 'Y'</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>로</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>변경처리</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">, </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>삭제사유를</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>남기기</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>위해</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>보관처리</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -4028,7 +4306,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="182">
   <si>
     <t>비고</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4094,35 +4372,155 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>NOT NULL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRIMARY KEY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연락처</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>질문답</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>img</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FOREIGN KEY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zipcode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우편번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>NUMBER</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NOT NULL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRIMARY KEY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아이디</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>연락처</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>질문답</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>img</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FOREIGN KEY</t>
+    <t>문의사항</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알림</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스터디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>좋아하는 스터디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스터디 참여자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스터디 신청자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지사항</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스터디 댓글</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스터디 공지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스터디 공지 댓글</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>input_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view_cnt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLOB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내용</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -4130,19 +4528,335 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>subject</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>제목</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNIQUE</t>
+    <t>조회수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>닉네임</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주소1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주소2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이메일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인증질문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소개글</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탈퇴여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가입일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nick</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addr1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addr2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>question</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>answer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deactivation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHAR(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>q_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>category</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>answer_flag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>answer_content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문의내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>답변여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>답변내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>읽음여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read_flag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>recruitment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스터디 코드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스터디명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지역</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상세설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모집여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>생성일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종료여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리더 아이디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>q_000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n_000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>accept_flag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수락여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신청일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRIMARY KEY, FOREIGN KEY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자기소개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지원동기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>introduce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>motive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글 등록일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스터디 공지 번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모임시간</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>작성일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sn_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>meeting_info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>workload</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>finish_flag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과제내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완료여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알림 번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지사항 번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문의번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a_000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLOB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -4150,191 +4864,167 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NOT NULL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>zipcode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>우편번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NUMBER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>문의사항</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>유저</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>알림</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스터디</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>좋아하는 스터디</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스터디 참여자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스터디 신청자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공지사항</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스터디 댓글</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스터디 공지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스터디 공지 댓글</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>과제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>n_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>input_date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>view_cnt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CLOB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>제목</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>등록일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>조회수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>닉네임</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>비밀번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>주소1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주소2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이메일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인증질문</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이미지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>소개글</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>탈퇴여부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>가입일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nick</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>addr1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>addr2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>question</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>answer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>deactivation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CHAR(1)</t>
+    <t>관리자 아이디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 유저</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>notice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alarm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin_user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>join</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fav_study</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study_notice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>homework</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity : notice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity : question</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity : alarm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity : admin_user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity : study</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity : member</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity : join</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity : fav_study</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity : study_notice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity : homework</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PK, FK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity : sn_comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity : s_comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sn_comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity : user_table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_code 함수를 사용해서 번호 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n_code 함수를 사용해서 번호 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>q_code 함수를 사용해서 번호 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a_code 함수를 사용해서 번호 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_code 함수를 사용해서 번호 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sn_000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sn_code 함수를 사용해서 번호 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삭제여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete_flag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>answer_date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -4342,403 +5032,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>q_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>category</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>answer_flag</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>answer_content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>분류</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>문의내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>답변여부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>답변내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>읽음여부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>read_flag</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>study_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>loc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>recruitment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CHAR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스터디 코드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스터디명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지역</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상세설명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>모집여부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>생성일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>종료여부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>리더 아이디</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>q_000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>n_000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s_000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>accept_flag</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수락여부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>신청일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRIMARY KEY, FOREIGN KEY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자기소개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지원동기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>introduce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>motive</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>comment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>댓글내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>댓글 등록일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스터디 공지 번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공지명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>모임시간</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>작성일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sn_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>meeting_info</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>addr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>workload</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>finish_flag</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>과제내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>완료여부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>알림 번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공지사항 번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>문의번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a_000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CLOB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공지내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>비밀번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자 아이디</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자 유저</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>notice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>alarm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>admin_user</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>study</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>member</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>join</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fav_study</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>study_notice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>homework</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity : notice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity : question</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity : alarm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity : admin_user</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity : study</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity : member</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity : join</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity : fav_study</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity : study_notice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity : homework</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PK, FK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s_comment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity : sn_comment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity : s_comment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sn_comment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity : user_table</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user_table</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user_code 함수를 사용해서 번호 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>n_code 함수를 사용해서 번호 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>q_code 함수를 사용해서 번호 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a_code 함수를 사용해서 번호 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s_code 함수를 사용해서 번호 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sn_000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sn_code 함수를 사용해서 번호 생성</t>
+    <t>답변일</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5192,7 +5486,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -5213,10 +5507,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -5224,10 +5518,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -5235,10 +5529,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -5246,10 +5540,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -5257,10 +5551,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -5268,10 +5562,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -5279,10 +5573,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -5290,10 +5584,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -5301,10 +5595,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -5312,10 +5606,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -5323,10 +5617,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -5334,10 +5628,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -5345,10 +5639,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -5380,7 +5674,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -5417,7 +5711,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>15</v>
@@ -5426,13 +5720,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5443,19 +5737,19 @@
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3">
         <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -5483,7 +5777,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -5520,20 +5814,20 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3">
         <v>300</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5541,18 +5835,18 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5563,19 +5857,19 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3">
         <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5583,7 +5877,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>15</v>
@@ -5592,13 +5886,13 @@
         <v>8</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -5627,7 +5921,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -5664,7 +5958,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>15</v>
@@ -5673,13 +5967,13 @@
         <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5687,20 +5981,20 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3">
         <v>300</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5708,20 +6002,20 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3">
         <v>100</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5729,20 +6023,20 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -5750,20 +6044,20 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="3">
         <v>300</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5771,7 +6065,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>15</v>
@@ -5780,13 +6074,13 @@
         <v>8</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -5794,28 +6088,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="B12" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -5844,7 +6138,7 @@
   <sheetData>
     <row r="1" spans="9:15">
       <c r="I1" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -5881,20 +6175,20 @@
         <v>1</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L3" s="3">
         <v>300</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="9:15">
@@ -5902,18 +6196,18 @@
         <v>2</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="9:15">
@@ -5924,19 +6218,19 @@
         <v>10</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L5" s="3">
         <v>15</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="9:15">
@@ -5944,7 +6238,7 @@
         <v>4</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>15</v>
@@ -5953,13 +6247,13 @@
         <v>9</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -5988,7 +6282,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6028,19 +6322,19 @@
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3">
         <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6048,20 +6342,20 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3">
         <v>300</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6069,7 +6363,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>15</v>
@@ -6080,7 +6374,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -6088,22 +6382,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" s="3">
         <v>9</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -6133,7 +6427,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6170,7 +6464,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>15</v>
@@ -6179,13 +6473,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -6193,20 +6487,20 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3">
         <v>300</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -6214,20 +6508,20 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -6235,18 +6529,18 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -6254,28 +6548,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="B9" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="B10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -6293,8 +6587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -6306,7 +6600,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6352,13 +6646,13 @@
         <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6366,7 +6660,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
@@ -6376,10 +6670,10 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6387,7 +6681,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>14</v>
@@ -6396,11 +6690,11 @@
         <v>30</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -6408,20 +6702,20 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="3">
         <v>100</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -6429,20 +6723,20 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="3">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -6450,20 +6744,20 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="3">
         <v>150</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -6471,20 +6765,20 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="3">
         <v>150</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6495,17 +6789,17 @@
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="3">
         <v>13</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -6522,13 +6816,13 @@
         <v>100</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -6536,20 +6830,20 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -6557,20 +6851,20 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" s="3">
         <v>100</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -6578,7 +6872,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>14</v>
@@ -6589,7 +6883,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -6597,10 +6891,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="3">
         <v>300</v>
@@ -6608,7 +6902,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -6616,7 +6910,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>15</v>
@@ -6627,7 +6921,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -6635,7 +6929,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>13</v>
@@ -6644,17 +6938,17 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="B21" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="B22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -6681,8 +6975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -6696,7 +6990,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6733,7 +7027,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>15</v>
@@ -6742,13 +7036,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6756,20 +7050,20 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3">
         <v>300</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6777,20 +7071,20 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3">
         <v>12</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -6798,20 +7092,20 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -6819,18 +7113,18 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -6838,7 +7132,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>15</v>
@@ -6849,7 +7143,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -6857,18 +7151,18 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6879,29 +7173,50 @@
         <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="3">
         <v>15</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="B14" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="B15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -6929,7 +7244,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6966,20 +7281,20 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3">
         <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6987,20 +7302,20 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3">
         <v>300</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7008,20 +7323,20 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3">
         <v>300</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -7029,18 +7344,18 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -7048,7 +7363,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>15</v>
@@ -7059,7 +7374,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -7070,19 +7385,19 @@
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="3">
         <v>15</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -7090,7 +7405,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>15</v>
@@ -7099,23 +7414,23 @@
         <v>8</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="G9" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="B14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -7145,7 +7460,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -7180,22 +7495,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3">
         <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -7203,20 +7518,20 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3">
         <v>100</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7224,20 +7539,20 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -7252,7 +7567,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -7265,7 +7580,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -7302,7 +7617,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>15</v>
@@ -7311,13 +7626,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -7325,22 +7640,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3">
         <v>72</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7348,20 +7663,20 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" s="3">
         <v>6</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -7369,20 +7684,20 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -7390,20 +7705,20 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -7411,10 +7726,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="3">
         <v>100</v>
@@ -7422,7 +7737,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -7430,7 +7745,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>15</v>
@@ -7441,7 +7756,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -7449,18 +7764,18 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -7468,7 +7783,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>15</v>
@@ -7479,7 +7794,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -7490,19 +7805,19 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="3">
         <v>15</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -7510,7 +7825,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>15</v>
@@ -7521,23 +7836,43 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="3">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7559,7 +7894,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -7599,19 +7934,19 @@
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3">
         <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -7619,7 +7954,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>15</v>
@@ -7628,13 +7963,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -7662,7 +7997,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -7702,19 +8037,19 @@
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3">
         <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -7722,7 +8057,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>15</v>
@@ -7731,13 +8066,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7745,20 +8080,20 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3">
         <v>300</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -7766,20 +8101,20 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="3">
         <v>300</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -7787,7 +8122,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>15</v>
@@ -7798,7 +8133,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -7806,20 +8141,20 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>